<commit_message>
nueva sección templates para bodas productos
</commit_message>
<xml_diff>
--- a/static/data/price_tiers_complete.xlsx
+++ b/static/data/price_tiers_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A504A7C8-5707-4249-8BE0-7890B185672F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BB11D0-C02D-4295-9E91-8F44C4F97B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="186">
   <si>
     <t>product_slug</t>
   </si>
@@ -574,121 +574,10 @@
     <t>district-r-women-s-racerback-tank-top-heat-transfer</t>
   </si>
   <si>
-    <t>stationery-wedding-invitations_0002</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0003</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0004</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0005</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0006</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0007</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0008</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0009</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0010</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0011</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0012</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0013</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0014</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0015</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0016</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0017</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0018</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0019</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0020</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0021</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0022</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0023</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0024</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0025</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0026</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0027</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0028</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0029</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0030</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0031</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0032</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0033</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0034</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0035</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0036</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0037</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0038</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0039</t>
-  </si>
-  <si>
-    <t>stationery-wedding-invitations_0040</t>
+    <t>guarda-la-fecha</t>
+  </si>
+  <si>
+    <t>servilletas</t>
   </si>
 </sst>
 </file>
@@ -1535,9 +1424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1091"/>
+  <dimension ref="A1:E906"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A875" workbookViewId="0">
+      <selection activeCell="H895" sqref="H895"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -16946,3151 +16837,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="907" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A907" t="s">
-        <v>186</v>
-      </c>
-      <c r="B907">
-        <v>1</v>
-      </c>
-      <c r="C907">
-        <v>49</v>
-      </c>
-      <c r="D907">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E907">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="908" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A908" t="s">
-        <v>186</v>
-      </c>
-      <c r="B908">
-        <v>50</v>
-      </c>
-      <c r="C908">
-        <v>99</v>
-      </c>
-      <c r="D908">
-        <v>1.83</v>
-      </c>
-      <c r="E908">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="909" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A909" t="s">
-        <v>186</v>
-      </c>
-      <c r="B909">
-        <v>100</v>
-      </c>
-      <c r="C909">
-        <v>249</v>
-      </c>
-      <c r="D909">
-        <v>1.47</v>
-      </c>
-      <c r="E909">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="910" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A910" t="s">
-        <v>186</v>
-      </c>
-      <c r="B910">
-        <v>250</v>
-      </c>
-      <c r="C910">
-        <v>499</v>
-      </c>
-      <c r="D910">
-        <v>1.19</v>
-      </c>
-      <c r="E910">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="911" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A911" t="s">
-        <v>186</v>
-      </c>
-      <c r="B911">
-        <v>500</v>
-      </c>
-      <c r="C911">
-        <v>999999</v>
-      </c>
-      <c r="D911">
-        <v>0.92</v>
-      </c>
-      <c r="E911">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="912" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A912" t="s">
-        <v>187</v>
-      </c>
-      <c r="B912">
-        <v>1</v>
-      </c>
-      <c r="C912">
-        <v>49</v>
-      </c>
-      <c r="D912">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E912">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="913" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A913" t="s">
-        <v>187</v>
-      </c>
-      <c r="B913">
-        <v>50</v>
-      </c>
-      <c r="C913">
-        <v>99</v>
-      </c>
-      <c r="D913">
-        <v>1.83</v>
-      </c>
-      <c r="E913">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="914" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A914" t="s">
-        <v>187</v>
-      </c>
-      <c r="B914">
-        <v>100</v>
-      </c>
-      <c r="C914">
-        <v>249</v>
-      </c>
-      <c r="D914">
-        <v>1.47</v>
-      </c>
-      <c r="E914">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="915" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A915" t="s">
-        <v>187</v>
-      </c>
-      <c r="B915">
-        <v>250</v>
-      </c>
-      <c r="C915">
-        <v>499</v>
-      </c>
-      <c r="D915">
-        <v>1.19</v>
-      </c>
-      <c r="E915">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="916" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A916" t="s">
-        <v>187</v>
-      </c>
-      <c r="B916">
-        <v>500</v>
-      </c>
-      <c r="C916">
-        <v>999999</v>
-      </c>
-      <c r="D916">
-        <v>0.92</v>
-      </c>
-      <c r="E916">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="917" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A917" t="s">
-        <v>188</v>
-      </c>
-      <c r="B917">
-        <v>1</v>
-      </c>
-      <c r="C917">
-        <v>49</v>
-      </c>
-      <c r="D917">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E917">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="918" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A918" t="s">
-        <v>188</v>
-      </c>
-      <c r="B918">
-        <v>50</v>
-      </c>
-      <c r="C918">
-        <v>99</v>
-      </c>
-      <c r="D918">
-        <v>1.83</v>
-      </c>
-      <c r="E918">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="919" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A919" t="s">
-        <v>188</v>
-      </c>
-      <c r="B919">
-        <v>100</v>
-      </c>
-      <c r="C919">
-        <v>249</v>
-      </c>
-      <c r="D919">
-        <v>1.47</v>
-      </c>
-      <c r="E919">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="920" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A920" t="s">
-        <v>188</v>
-      </c>
-      <c r="B920">
-        <v>250</v>
-      </c>
-      <c r="C920">
-        <v>499</v>
-      </c>
-      <c r="D920">
-        <v>1.19</v>
-      </c>
-      <c r="E920">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="921" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A921" t="s">
-        <v>188</v>
-      </c>
-      <c r="B921">
-        <v>500</v>
-      </c>
-      <c r="C921">
-        <v>999999</v>
-      </c>
-      <c r="D921">
-        <v>0.92</v>
-      </c>
-      <c r="E921">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="922" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A922" t="s">
-        <v>189</v>
-      </c>
-      <c r="B922">
-        <v>1</v>
-      </c>
-      <c r="C922">
-        <v>49</v>
-      </c>
-      <c r="D922">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E922">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="923" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A923" t="s">
-        <v>189</v>
-      </c>
-      <c r="B923">
-        <v>50</v>
-      </c>
-      <c r="C923">
-        <v>99</v>
-      </c>
-      <c r="D923">
-        <v>1.83</v>
-      </c>
-      <c r="E923">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="924" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A924" t="s">
-        <v>189</v>
-      </c>
-      <c r="B924">
-        <v>100</v>
-      </c>
-      <c r="C924">
-        <v>249</v>
-      </c>
-      <c r="D924">
-        <v>1.47</v>
-      </c>
-      <c r="E924">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="925" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A925" t="s">
-        <v>189</v>
-      </c>
-      <c r="B925">
-        <v>250</v>
-      </c>
-      <c r="C925">
-        <v>499</v>
-      </c>
-      <c r="D925">
-        <v>1.19</v>
-      </c>
-      <c r="E925">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="926" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A926" t="s">
-        <v>189</v>
-      </c>
-      <c r="B926">
-        <v>500</v>
-      </c>
-      <c r="C926">
-        <v>999999</v>
-      </c>
-      <c r="D926">
-        <v>0.92</v>
-      </c>
-      <c r="E926">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="927" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A927" t="s">
-        <v>190</v>
-      </c>
-      <c r="B927">
-        <v>1</v>
-      </c>
-      <c r="C927">
-        <v>49</v>
-      </c>
-      <c r="D927">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E927">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="928" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A928" t="s">
-        <v>190</v>
-      </c>
-      <c r="B928">
-        <v>50</v>
-      </c>
-      <c r="C928">
-        <v>99</v>
-      </c>
-      <c r="D928">
-        <v>1.83</v>
-      </c>
-      <c r="E928">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="929" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A929" t="s">
-        <v>190</v>
-      </c>
-      <c r="B929">
-        <v>100</v>
-      </c>
-      <c r="C929">
-        <v>249</v>
-      </c>
-      <c r="D929">
-        <v>1.47</v>
-      </c>
-      <c r="E929">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="930" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A930" t="s">
-        <v>190</v>
-      </c>
-      <c r="B930">
-        <v>250</v>
-      </c>
-      <c r="C930">
-        <v>499</v>
-      </c>
-      <c r="D930">
-        <v>1.19</v>
-      </c>
-      <c r="E930">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="931" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A931" t="s">
-        <v>190</v>
-      </c>
-      <c r="B931">
-        <v>500</v>
-      </c>
-      <c r="C931">
-        <v>999999</v>
-      </c>
-      <c r="D931">
-        <v>0.92</v>
-      </c>
-      <c r="E931">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="932" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A932" t="s">
-        <v>191</v>
-      </c>
-      <c r="B932">
-        <v>1</v>
-      </c>
-      <c r="C932">
-        <v>49</v>
-      </c>
-      <c r="D932">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E932">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="933" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A933" t="s">
-        <v>191</v>
-      </c>
-      <c r="B933">
-        <v>50</v>
-      </c>
-      <c r="C933">
-        <v>99</v>
-      </c>
-      <c r="D933">
-        <v>1.83</v>
-      </c>
-      <c r="E933">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="934" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A934" t="s">
-        <v>191</v>
-      </c>
-      <c r="B934">
-        <v>100</v>
-      </c>
-      <c r="C934">
-        <v>249</v>
-      </c>
-      <c r="D934">
-        <v>1.47</v>
-      </c>
-      <c r="E934">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="935" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A935" t="s">
-        <v>191</v>
-      </c>
-      <c r="B935">
-        <v>250</v>
-      </c>
-      <c r="C935">
-        <v>499</v>
-      </c>
-      <c r="D935">
-        <v>1.19</v>
-      </c>
-      <c r="E935">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="936" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A936" t="s">
-        <v>191</v>
-      </c>
-      <c r="B936">
-        <v>500</v>
-      </c>
-      <c r="C936">
-        <v>999999</v>
-      </c>
-      <c r="D936">
-        <v>0.92</v>
-      </c>
-      <c r="E936">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="937" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A937" t="s">
-        <v>192</v>
-      </c>
-      <c r="B937">
-        <v>1</v>
-      </c>
-      <c r="C937">
-        <v>49</v>
-      </c>
-      <c r="D937">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E937">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="938" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A938" t="s">
-        <v>192</v>
-      </c>
-      <c r="B938">
-        <v>50</v>
-      </c>
-      <c r="C938">
-        <v>99</v>
-      </c>
-      <c r="D938">
-        <v>1.83</v>
-      </c>
-      <c r="E938">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="939" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A939" t="s">
-        <v>192</v>
-      </c>
-      <c r="B939">
-        <v>100</v>
-      </c>
-      <c r="C939">
-        <v>249</v>
-      </c>
-      <c r="D939">
-        <v>1.47</v>
-      </c>
-      <c r="E939">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="940" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A940" t="s">
-        <v>192</v>
-      </c>
-      <c r="B940">
-        <v>250</v>
-      </c>
-      <c r="C940">
-        <v>499</v>
-      </c>
-      <c r="D940">
-        <v>1.19</v>
-      </c>
-      <c r="E940">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="941" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A941" t="s">
-        <v>192</v>
-      </c>
-      <c r="B941">
-        <v>500</v>
-      </c>
-      <c r="C941">
-        <v>999999</v>
-      </c>
-      <c r="D941">
-        <v>0.92</v>
-      </c>
-      <c r="E941">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="942" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A942" t="s">
-        <v>193</v>
-      </c>
-      <c r="B942">
-        <v>1</v>
-      </c>
-      <c r="C942">
-        <v>49</v>
-      </c>
-      <c r="D942">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E942">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="943" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A943" t="s">
-        <v>193</v>
-      </c>
-      <c r="B943">
-        <v>50</v>
-      </c>
-      <c r="C943">
-        <v>99</v>
-      </c>
-      <c r="D943">
-        <v>1.83</v>
-      </c>
-      <c r="E943">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="944" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A944" t="s">
-        <v>193</v>
-      </c>
-      <c r="B944">
-        <v>100</v>
-      </c>
-      <c r="C944">
-        <v>249</v>
-      </c>
-      <c r="D944">
-        <v>1.47</v>
-      </c>
-      <c r="E944">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="945" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A945" t="s">
-        <v>193</v>
-      </c>
-      <c r="B945">
-        <v>250</v>
-      </c>
-      <c r="C945">
-        <v>499</v>
-      </c>
-      <c r="D945">
-        <v>1.19</v>
-      </c>
-      <c r="E945">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="946" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A946" t="s">
-        <v>193</v>
-      </c>
-      <c r="B946">
-        <v>500</v>
-      </c>
-      <c r="C946">
-        <v>999999</v>
-      </c>
-      <c r="D946">
-        <v>0.92</v>
-      </c>
-      <c r="E946">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="947" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A947" t="s">
-        <v>194</v>
-      </c>
-      <c r="B947">
-        <v>1</v>
-      </c>
-      <c r="C947">
-        <v>49</v>
-      </c>
-      <c r="D947">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E947">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="948" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A948" t="s">
-        <v>194</v>
-      </c>
-      <c r="B948">
-        <v>50</v>
-      </c>
-      <c r="C948">
-        <v>99</v>
-      </c>
-      <c r="D948">
-        <v>1.83</v>
-      </c>
-      <c r="E948">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="949" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A949" t="s">
-        <v>194</v>
-      </c>
-      <c r="B949">
-        <v>100</v>
-      </c>
-      <c r="C949">
-        <v>249</v>
-      </c>
-      <c r="D949">
-        <v>1.47</v>
-      </c>
-      <c r="E949">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="950" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A950" t="s">
-        <v>194</v>
-      </c>
-      <c r="B950">
-        <v>250</v>
-      </c>
-      <c r="C950">
-        <v>499</v>
-      </c>
-      <c r="D950">
-        <v>1.19</v>
-      </c>
-      <c r="E950">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="951" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A951" t="s">
-        <v>194</v>
-      </c>
-      <c r="B951">
-        <v>500</v>
-      </c>
-      <c r="C951">
-        <v>999999</v>
-      </c>
-      <c r="D951">
-        <v>0.92</v>
-      </c>
-      <c r="E951">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="952" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A952" t="s">
-        <v>195</v>
-      </c>
-      <c r="B952">
-        <v>1</v>
-      </c>
-      <c r="C952">
-        <v>49</v>
-      </c>
-      <c r="D952">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E952">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="953" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A953" t="s">
-        <v>195</v>
-      </c>
-      <c r="B953">
-        <v>50</v>
-      </c>
-      <c r="C953">
-        <v>99</v>
-      </c>
-      <c r="D953">
-        <v>1.83</v>
-      </c>
-      <c r="E953">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="954" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A954" t="s">
-        <v>195</v>
-      </c>
-      <c r="B954">
-        <v>100</v>
-      </c>
-      <c r="C954">
-        <v>249</v>
-      </c>
-      <c r="D954">
-        <v>1.47</v>
-      </c>
-      <c r="E954">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="955" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A955" t="s">
-        <v>195</v>
-      </c>
-      <c r="B955">
-        <v>250</v>
-      </c>
-      <c r="C955">
-        <v>499</v>
-      </c>
-      <c r="D955">
-        <v>1.19</v>
-      </c>
-      <c r="E955">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="956" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A956" t="s">
-        <v>195</v>
-      </c>
-      <c r="B956">
-        <v>500</v>
-      </c>
-      <c r="C956">
-        <v>999999</v>
-      </c>
-      <c r="D956">
-        <v>0.92</v>
-      </c>
-      <c r="E956">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="957" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A957" t="s">
-        <v>196</v>
-      </c>
-      <c r="B957">
-        <v>1</v>
-      </c>
-      <c r="C957">
-        <v>49</v>
-      </c>
-      <c r="D957">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E957">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="958" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A958" t="s">
-        <v>196</v>
-      </c>
-      <c r="B958">
-        <v>50</v>
-      </c>
-      <c r="C958">
-        <v>99</v>
-      </c>
-      <c r="D958">
-        <v>1.83</v>
-      </c>
-      <c r="E958">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="959" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A959" t="s">
-        <v>196</v>
-      </c>
-      <c r="B959">
-        <v>100</v>
-      </c>
-      <c r="C959">
-        <v>249</v>
-      </c>
-      <c r="D959">
-        <v>1.47</v>
-      </c>
-      <c r="E959">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="960" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A960" t="s">
-        <v>196</v>
-      </c>
-      <c r="B960">
-        <v>250</v>
-      </c>
-      <c r="C960">
-        <v>499</v>
-      </c>
-      <c r="D960">
-        <v>1.19</v>
-      </c>
-      <c r="E960">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="961" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A961" t="s">
-        <v>196</v>
-      </c>
-      <c r="B961">
-        <v>500</v>
-      </c>
-      <c r="C961">
-        <v>999999</v>
-      </c>
-      <c r="D961">
-        <v>0.92</v>
-      </c>
-      <c r="E961">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="962" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A962" t="s">
-        <v>197</v>
-      </c>
-      <c r="B962">
-        <v>1</v>
-      </c>
-      <c r="C962">
-        <v>49</v>
-      </c>
-      <c r="D962">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E962">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="963" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A963" t="s">
-        <v>197</v>
-      </c>
-      <c r="B963">
-        <v>50</v>
-      </c>
-      <c r="C963">
-        <v>99</v>
-      </c>
-      <c r="D963">
-        <v>1.83</v>
-      </c>
-      <c r="E963">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="964" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A964" t="s">
-        <v>197</v>
-      </c>
-      <c r="B964">
-        <v>100</v>
-      </c>
-      <c r="C964">
-        <v>249</v>
-      </c>
-      <c r="D964">
-        <v>1.47</v>
-      </c>
-      <c r="E964">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="965" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A965" t="s">
-        <v>197</v>
-      </c>
-      <c r="B965">
-        <v>250</v>
-      </c>
-      <c r="C965">
-        <v>499</v>
-      </c>
-      <c r="D965">
-        <v>1.19</v>
-      </c>
-      <c r="E965">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="966" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A966" t="s">
-        <v>197</v>
-      </c>
-      <c r="B966">
-        <v>500</v>
-      </c>
-      <c r="C966">
-        <v>999999</v>
-      </c>
-      <c r="D966">
-        <v>0.92</v>
-      </c>
-      <c r="E966">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="967" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A967" t="s">
-        <v>198</v>
-      </c>
-      <c r="B967">
-        <v>1</v>
-      </c>
-      <c r="C967">
-        <v>49</v>
-      </c>
-      <c r="D967">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E967">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="968" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A968" t="s">
-        <v>198</v>
-      </c>
-      <c r="B968">
-        <v>50</v>
-      </c>
-      <c r="C968">
-        <v>99</v>
-      </c>
-      <c r="D968">
-        <v>1.83</v>
-      </c>
-      <c r="E968">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="969" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A969" t="s">
-        <v>198</v>
-      </c>
-      <c r="B969">
-        <v>100</v>
-      </c>
-      <c r="C969">
-        <v>249</v>
-      </c>
-      <c r="D969">
-        <v>1.47</v>
-      </c>
-      <c r="E969">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="970" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A970" t="s">
-        <v>198</v>
-      </c>
-      <c r="B970">
-        <v>250</v>
-      </c>
-      <c r="C970">
-        <v>499</v>
-      </c>
-      <c r="D970">
-        <v>1.19</v>
-      </c>
-      <c r="E970">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="971" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A971" t="s">
-        <v>198</v>
-      </c>
-      <c r="B971">
-        <v>500</v>
-      </c>
-      <c r="C971">
-        <v>999999</v>
-      </c>
-      <c r="D971">
-        <v>0.92</v>
-      </c>
-      <c r="E971">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="972" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A972" t="s">
-        <v>199</v>
-      </c>
-      <c r="B972">
-        <v>1</v>
-      </c>
-      <c r="C972">
-        <v>49</v>
-      </c>
-      <c r="D972">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E972">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="973" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A973" t="s">
-        <v>199</v>
-      </c>
-      <c r="B973">
-        <v>50</v>
-      </c>
-      <c r="C973">
-        <v>99</v>
-      </c>
-      <c r="D973">
-        <v>1.83</v>
-      </c>
-      <c r="E973">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="974" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A974" t="s">
-        <v>199</v>
-      </c>
-      <c r="B974">
-        <v>100</v>
-      </c>
-      <c r="C974">
-        <v>249</v>
-      </c>
-      <c r="D974">
-        <v>1.47</v>
-      </c>
-      <c r="E974">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="975" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A975" t="s">
-        <v>199</v>
-      </c>
-      <c r="B975">
-        <v>250</v>
-      </c>
-      <c r="C975">
-        <v>499</v>
-      </c>
-      <c r="D975">
-        <v>1.19</v>
-      </c>
-      <c r="E975">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="976" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A976" t="s">
-        <v>199</v>
-      </c>
-      <c r="B976">
-        <v>500</v>
-      </c>
-      <c r="C976">
-        <v>999999</v>
-      </c>
-      <c r="D976">
-        <v>0.92</v>
-      </c>
-      <c r="E976">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="977" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A977" t="s">
-        <v>200</v>
-      </c>
-      <c r="B977">
-        <v>1</v>
-      </c>
-      <c r="C977">
-        <v>49</v>
-      </c>
-      <c r="D977">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E977">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="978" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A978" t="s">
-        <v>200</v>
-      </c>
-      <c r="B978">
-        <v>50</v>
-      </c>
-      <c r="C978">
-        <v>99</v>
-      </c>
-      <c r="D978">
-        <v>1.83</v>
-      </c>
-      <c r="E978">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="979" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A979" t="s">
-        <v>200</v>
-      </c>
-      <c r="B979">
-        <v>100</v>
-      </c>
-      <c r="C979">
-        <v>249</v>
-      </c>
-      <c r="D979">
-        <v>1.47</v>
-      </c>
-      <c r="E979">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="980" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A980" t="s">
-        <v>200</v>
-      </c>
-      <c r="B980">
-        <v>250</v>
-      </c>
-      <c r="C980">
-        <v>499</v>
-      </c>
-      <c r="D980">
-        <v>1.19</v>
-      </c>
-      <c r="E980">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="981" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A981" t="s">
-        <v>200</v>
-      </c>
-      <c r="B981">
-        <v>500</v>
-      </c>
-      <c r="C981">
-        <v>999999</v>
-      </c>
-      <c r="D981">
-        <v>0.92</v>
-      </c>
-      <c r="E981">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="982" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A982" t="s">
-        <v>201</v>
-      </c>
-      <c r="B982">
-        <v>1</v>
-      </c>
-      <c r="C982">
-        <v>49</v>
-      </c>
-      <c r="D982">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E982">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="983" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A983" t="s">
-        <v>201</v>
-      </c>
-      <c r="B983">
-        <v>50</v>
-      </c>
-      <c r="C983">
-        <v>99</v>
-      </c>
-      <c r="D983">
-        <v>1.83</v>
-      </c>
-      <c r="E983">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="984" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A984" t="s">
-        <v>201</v>
-      </c>
-      <c r="B984">
-        <v>100</v>
-      </c>
-      <c r="C984">
-        <v>249</v>
-      </c>
-      <c r="D984">
-        <v>1.47</v>
-      </c>
-      <c r="E984">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="985" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A985" t="s">
-        <v>201</v>
-      </c>
-      <c r="B985">
-        <v>250</v>
-      </c>
-      <c r="C985">
-        <v>499</v>
-      </c>
-      <c r="D985">
-        <v>1.19</v>
-      </c>
-      <c r="E985">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="986" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A986" t="s">
-        <v>201</v>
-      </c>
-      <c r="B986">
-        <v>500</v>
-      </c>
-      <c r="C986">
-        <v>999999</v>
-      </c>
-      <c r="D986">
-        <v>0.92</v>
-      </c>
-      <c r="E986">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="987" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A987" t="s">
-        <v>202</v>
-      </c>
-      <c r="B987">
-        <v>1</v>
-      </c>
-      <c r="C987">
-        <v>49</v>
-      </c>
-      <c r="D987">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E987">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="988" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A988" t="s">
-        <v>202</v>
-      </c>
-      <c r="B988">
-        <v>50</v>
-      </c>
-      <c r="C988">
-        <v>99</v>
-      </c>
-      <c r="D988">
-        <v>1.83</v>
-      </c>
-      <c r="E988">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="989" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A989" t="s">
-        <v>202</v>
-      </c>
-      <c r="B989">
-        <v>100</v>
-      </c>
-      <c r="C989">
-        <v>249</v>
-      </c>
-      <c r="D989">
-        <v>1.47</v>
-      </c>
-      <c r="E989">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="990" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A990" t="s">
-        <v>202</v>
-      </c>
-      <c r="B990">
-        <v>250</v>
-      </c>
-      <c r="C990">
-        <v>499</v>
-      </c>
-      <c r="D990">
-        <v>1.19</v>
-      </c>
-      <c r="E990">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="991" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A991" t="s">
-        <v>202</v>
-      </c>
-      <c r="B991">
-        <v>500</v>
-      </c>
-      <c r="C991">
-        <v>999999</v>
-      </c>
-      <c r="D991">
-        <v>0.92</v>
-      </c>
-      <c r="E991">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="992" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A992" t="s">
-        <v>203</v>
-      </c>
-      <c r="B992">
-        <v>1</v>
-      </c>
-      <c r="C992">
-        <v>49</v>
-      </c>
-      <c r="D992">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E992">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="993" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A993" t="s">
-        <v>203</v>
-      </c>
-      <c r="B993">
-        <v>50</v>
-      </c>
-      <c r="C993">
-        <v>99</v>
-      </c>
-      <c r="D993">
-        <v>1.83</v>
-      </c>
-      <c r="E993">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="994" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A994" t="s">
-        <v>203</v>
-      </c>
-      <c r="B994">
-        <v>100</v>
-      </c>
-      <c r="C994">
-        <v>249</v>
-      </c>
-      <c r="D994">
-        <v>1.47</v>
-      </c>
-      <c r="E994">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="995" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A995" t="s">
-        <v>203</v>
-      </c>
-      <c r="B995">
-        <v>250</v>
-      </c>
-      <c r="C995">
-        <v>499</v>
-      </c>
-      <c r="D995">
-        <v>1.19</v>
-      </c>
-      <c r="E995">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="996" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A996" t="s">
-        <v>203</v>
-      </c>
-      <c r="B996">
-        <v>500</v>
-      </c>
-      <c r="C996">
-        <v>999999</v>
-      </c>
-      <c r="D996">
-        <v>0.92</v>
-      </c>
-      <c r="E996">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="997" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A997" t="s">
-        <v>204</v>
-      </c>
-      <c r="B997">
-        <v>1</v>
-      </c>
-      <c r="C997">
-        <v>49</v>
-      </c>
-      <c r="D997">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E997">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="998" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A998" t="s">
-        <v>204</v>
-      </c>
-      <c r="B998">
-        <v>50</v>
-      </c>
-      <c r="C998">
-        <v>99</v>
-      </c>
-      <c r="D998">
-        <v>1.83</v>
-      </c>
-      <c r="E998">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="999" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A999" t="s">
-        <v>204</v>
-      </c>
-      <c r="B999">
-        <v>100</v>
-      </c>
-      <c r="C999">
-        <v>249</v>
-      </c>
-      <c r="D999">
-        <v>1.47</v>
-      </c>
-      <c r="E999">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1000" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1000" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1000">
-        <v>250</v>
-      </c>
-      <c r="C1000">
-        <v>499</v>
-      </c>
-      <c r="D1000">
-        <v>1.19</v>
-      </c>
-      <c r="E1000">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1001" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1001" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1001">
-        <v>500</v>
-      </c>
-      <c r="C1001">
-        <v>999999</v>
-      </c>
-      <c r="D1001">
-        <v>0.92</v>
-      </c>
-      <c r="E1001">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1002" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1002" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1002">
-        <v>1</v>
-      </c>
-      <c r="C1002">
-        <v>49</v>
-      </c>
-      <c r="D1002">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1002">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1003" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1003" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1003">
-        <v>50</v>
-      </c>
-      <c r="C1003">
-        <v>99</v>
-      </c>
-      <c r="D1003">
-        <v>1.83</v>
-      </c>
-      <c r="E1003">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1004" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1004">
-        <v>100</v>
-      </c>
-      <c r="C1004">
-        <v>249</v>
-      </c>
-      <c r="D1004">
-        <v>1.47</v>
-      </c>
-      <c r="E1004">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1005" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1005" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1005">
-        <v>250</v>
-      </c>
-      <c r="C1005">
-        <v>499</v>
-      </c>
-      <c r="D1005">
-        <v>1.19</v>
-      </c>
-      <c r="E1005">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1006" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1006" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1006">
-        <v>500</v>
-      </c>
-      <c r="C1006">
-        <v>999999</v>
-      </c>
-      <c r="D1006">
-        <v>0.92</v>
-      </c>
-      <c r="E1006">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1007" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1007" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1007">
-        <v>1</v>
-      </c>
-      <c r="C1007">
-        <v>49</v>
-      </c>
-      <c r="D1007">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1007">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1008" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1008" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1008">
-        <v>50</v>
-      </c>
-      <c r="C1008">
-        <v>99</v>
-      </c>
-      <c r="D1008">
-        <v>1.83</v>
-      </c>
-      <c r="E1008">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1009" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1009" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1009">
-        <v>100</v>
-      </c>
-      <c r="C1009">
-        <v>249</v>
-      </c>
-      <c r="D1009">
-        <v>1.47</v>
-      </c>
-      <c r="E1009">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1010" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1010" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1010">
-        <v>250</v>
-      </c>
-      <c r="C1010">
-        <v>499</v>
-      </c>
-      <c r="D1010">
-        <v>1.19</v>
-      </c>
-      <c r="E1010">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1011" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1011" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1011">
-        <v>500</v>
-      </c>
-      <c r="C1011">
-        <v>999999</v>
-      </c>
-      <c r="D1011">
-        <v>0.92</v>
-      </c>
-      <c r="E1011">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1012" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1012" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1012">
-        <v>1</v>
-      </c>
-      <c r="C1012">
-        <v>49</v>
-      </c>
-      <c r="D1012">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1012">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1013" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1013" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1013">
-        <v>50</v>
-      </c>
-      <c r="C1013">
-        <v>99</v>
-      </c>
-      <c r="D1013">
-        <v>1.83</v>
-      </c>
-      <c r="E1013">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1014" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1014">
-        <v>100</v>
-      </c>
-      <c r="C1014">
-        <v>249</v>
-      </c>
-      <c r="D1014">
-        <v>1.47</v>
-      </c>
-      <c r="E1014">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1015" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1015" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1015">
-        <v>250</v>
-      </c>
-      <c r="C1015">
-        <v>499</v>
-      </c>
-      <c r="D1015">
-        <v>1.19</v>
-      </c>
-      <c r="E1015">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1016" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1016">
-        <v>500</v>
-      </c>
-      <c r="C1016">
-        <v>999999</v>
-      </c>
-      <c r="D1016">
-        <v>0.92</v>
-      </c>
-      <c r="E1016">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1017" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1017">
-        <v>1</v>
-      </c>
-      <c r="C1017">
-        <v>49</v>
-      </c>
-      <c r="D1017">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1017">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1018" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1018">
-        <v>50</v>
-      </c>
-      <c r="C1018">
-        <v>99</v>
-      </c>
-      <c r="D1018">
-        <v>1.83</v>
-      </c>
-      <c r="E1018">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1019" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1019">
-        <v>100</v>
-      </c>
-      <c r="C1019">
-        <v>249</v>
-      </c>
-      <c r="D1019">
-        <v>1.47</v>
-      </c>
-      <c r="E1019">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1020" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1020">
-        <v>250</v>
-      </c>
-      <c r="C1020">
-        <v>499</v>
-      </c>
-      <c r="D1020">
-        <v>1.19</v>
-      </c>
-      <c r="E1020">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1021" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1021">
-        <v>500</v>
-      </c>
-      <c r="C1021">
-        <v>999999</v>
-      </c>
-      <c r="D1021">
-        <v>0.92</v>
-      </c>
-      <c r="E1021">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1022" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1022">
-        <v>1</v>
-      </c>
-      <c r="C1022">
-        <v>49</v>
-      </c>
-      <c r="D1022">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1022">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1023" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1023">
-        <v>50</v>
-      </c>
-      <c r="C1023">
-        <v>99</v>
-      </c>
-      <c r="D1023">
-        <v>1.83</v>
-      </c>
-      <c r="E1023">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1024" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1024">
-        <v>100</v>
-      </c>
-      <c r="C1024">
-        <v>249</v>
-      </c>
-      <c r="D1024">
-        <v>1.47</v>
-      </c>
-      <c r="E1024">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1025" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1025">
-        <v>250</v>
-      </c>
-      <c r="C1025">
-        <v>499</v>
-      </c>
-      <c r="D1025">
-        <v>1.19</v>
-      </c>
-      <c r="E1025">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1026" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1026">
-        <v>500</v>
-      </c>
-      <c r="C1026">
-        <v>999999</v>
-      </c>
-      <c r="D1026">
-        <v>0.92</v>
-      </c>
-      <c r="E1026">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1027" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1027">
-        <v>1</v>
-      </c>
-      <c r="C1027">
-        <v>49</v>
-      </c>
-      <c r="D1027">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1027">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1028" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1028">
-        <v>50</v>
-      </c>
-      <c r="C1028">
-        <v>99</v>
-      </c>
-      <c r="D1028">
-        <v>1.83</v>
-      </c>
-      <c r="E1028">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1029" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1029">
-        <v>100</v>
-      </c>
-      <c r="C1029">
-        <v>249</v>
-      </c>
-      <c r="D1029">
-        <v>1.47</v>
-      </c>
-      <c r="E1029">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1030" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1030">
-        <v>250</v>
-      </c>
-      <c r="C1030">
-        <v>499</v>
-      </c>
-      <c r="D1030">
-        <v>1.19</v>
-      </c>
-      <c r="E1030">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1031" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1031">
-        <v>500</v>
-      </c>
-      <c r="C1031">
-        <v>999999</v>
-      </c>
-      <c r="D1031">
-        <v>0.92</v>
-      </c>
-      <c r="E1031">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1032" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1032">
-        <v>1</v>
-      </c>
-      <c r="C1032">
-        <v>49</v>
-      </c>
-      <c r="D1032">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1032">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1033" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1033">
-        <v>50</v>
-      </c>
-      <c r="C1033">
-        <v>99</v>
-      </c>
-      <c r="D1033">
-        <v>1.83</v>
-      </c>
-      <c r="E1033">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1034" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1034">
-        <v>100</v>
-      </c>
-      <c r="C1034">
-        <v>249</v>
-      </c>
-      <c r="D1034">
-        <v>1.47</v>
-      </c>
-      <c r="E1034">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1035" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1035">
-        <v>250</v>
-      </c>
-      <c r="C1035">
-        <v>499</v>
-      </c>
-      <c r="D1035">
-        <v>1.19</v>
-      </c>
-      <c r="E1035">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1036" t="s">
-        <v>211</v>
-      </c>
-      <c r="B1036">
-        <v>500</v>
-      </c>
-      <c r="C1036">
-        <v>999999</v>
-      </c>
-      <c r="D1036">
-        <v>0.92</v>
-      </c>
-      <c r="E1036">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1037" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1037" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1037">
-        <v>1</v>
-      </c>
-      <c r="C1037">
-        <v>49</v>
-      </c>
-      <c r="D1037">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1037">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1038" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1038" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1038">
-        <v>50</v>
-      </c>
-      <c r="C1038">
-        <v>99</v>
-      </c>
-      <c r="D1038">
-        <v>1.83</v>
-      </c>
-      <c r="E1038">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1039" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1039">
-        <v>100</v>
-      </c>
-      <c r="C1039">
-        <v>249</v>
-      </c>
-      <c r="D1039">
-        <v>1.47</v>
-      </c>
-      <c r="E1039">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1040" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1040">
-        <v>250</v>
-      </c>
-      <c r="C1040">
-        <v>499</v>
-      </c>
-      <c r="D1040">
-        <v>1.19</v>
-      </c>
-      <c r="E1040">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1041" t="s">
-        <v>212</v>
-      </c>
-      <c r="B1041">
-        <v>500</v>
-      </c>
-      <c r="C1041">
-        <v>999999</v>
-      </c>
-      <c r="D1041">
-        <v>0.92</v>
-      </c>
-      <c r="E1041">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1042" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1042" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1042">
-        <v>1</v>
-      </c>
-      <c r="C1042">
-        <v>49</v>
-      </c>
-      <c r="D1042">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1042">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1043" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1043" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1043">
-        <v>50</v>
-      </c>
-      <c r="C1043">
-        <v>99</v>
-      </c>
-      <c r="D1043">
-        <v>1.83</v>
-      </c>
-      <c r="E1043">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1044" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1044" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1044">
-        <v>100</v>
-      </c>
-      <c r="C1044">
-        <v>249</v>
-      </c>
-      <c r="D1044">
-        <v>1.47</v>
-      </c>
-      <c r="E1044">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1045" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1045" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1045">
-        <v>250</v>
-      </c>
-      <c r="C1045">
-        <v>499</v>
-      </c>
-      <c r="D1045">
-        <v>1.19</v>
-      </c>
-      <c r="E1045">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1046" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1046" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1046">
-        <v>500</v>
-      </c>
-      <c r="C1046">
-        <v>999999</v>
-      </c>
-      <c r="D1046">
-        <v>0.92</v>
-      </c>
-      <c r="E1046">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1047" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1047" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1047">
-        <v>1</v>
-      </c>
-      <c r="C1047">
-        <v>49</v>
-      </c>
-      <c r="D1047">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1047">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1048" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1048">
-        <v>50</v>
-      </c>
-      <c r="C1048">
-        <v>99</v>
-      </c>
-      <c r="D1048">
-        <v>1.83</v>
-      </c>
-      <c r="E1048">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1049" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1049" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1049">
-        <v>100</v>
-      </c>
-      <c r="C1049">
-        <v>249</v>
-      </c>
-      <c r="D1049">
-        <v>1.47</v>
-      </c>
-      <c r="E1049">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1050" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1050" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1050">
-        <v>250</v>
-      </c>
-      <c r="C1050">
-        <v>499</v>
-      </c>
-      <c r="D1050">
-        <v>1.19</v>
-      </c>
-      <c r="E1050">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1051" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1051" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1051">
-        <v>500</v>
-      </c>
-      <c r="C1051">
-        <v>999999</v>
-      </c>
-      <c r="D1051">
-        <v>0.92</v>
-      </c>
-      <c r="E1051">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1052" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1052" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1052">
-        <v>1</v>
-      </c>
-      <c r="C1052">
-        <v>49</v>
-      </c>
-      <c r="D1052">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1052">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1053" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1053" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1053">
-        <v>50</v>
-      </c>
-      <c r="C1053">
-        <v>99</v>
-      </c>
-      <c r="D1053">
-        <v>1.83</v>
-      </c>
-      <c r="E1053">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1054" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1054" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1054">
-        <v>100</v>
-      </c>
-      <c r="C1054">
-        <v>249</v>
-      </c>
-      <c r="D1054">
-        <v>1.47</v>
-      </c>
-      <c r="E1054">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1055" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1055" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1055">
-        <v>250</v>
-      </c>
-      <c r="C1055">
-        <v>499</v>
-      </c>
-      <c r="D1055">
-        <v>1.19</v>
-      </c>
-      <c r="E1055">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1056" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1056" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1056">
-        <v>500</v>
-      </c>
-      <c r="C1056">
-        <v>999999</v>
-      </c>
-      <c r="D1056">
-        <v>0.92</v>
-      </c>
-      <c r="E1056">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1057" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1057" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1057">
-        <v>1</v>
-      </c>
-      <c r="C1057">
-        <v>49</v>
-      </c>
-      <c r="D1057">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1057">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1058" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1058" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1058">
-        <v>50</v>
-      </c>
-      <c r="C1058">
-        <v>99</v>
-      </c>
-      <c r="D1058">
-        <v>1.83</v>
-      </c>
-      <c r="E1058">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1059" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1059" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1059">
-        <v>100</v>
-      </c>
-      <c r="C1059">
-        <v>249</v>
-      </c>
-      <c r="D1059">
-        <v>1.47</v>
-      </c>
-      <c r="E1059">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1060" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1060">
-        <v>250</v>
-      </c>
-      <c r="C1060">
-        <v>499</v>
-      </c>
-      <c r="D1060">
-        <v>1.19</v>
-      </c>
-      <c r="E1060">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1061" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1061" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1061">
-        <v>500</v>
-      </c>
-      <c r="C1061">
-        <v>999999</v>
-      </c>
-      <c r="D1061">
-        <v>0.92</v>
-      </c>
-      <c r="E1061">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1062" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1062" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1062">
-        <v>1</v>
-      </c>
-      <c r="C1062">
-        <v>49</v>
-      </c>
-      <c r="D1062">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1062">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1063" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1063" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1063">
-        <v>50</v>
-      </c>
-      <c r="C1063">
-        <v>99</v>
-      </c>
-      <c r="D1063">
-        <v>1.83</v>
-      </c>
-      <c r="E1063">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1064" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1064">
-        <v>100</v>
-      </c>
-      <c r="C1064">
-        <v>249</v>
-      </c>
-      <c r="D1064">
-        <v>1.47</v>
-      </c>
-      <c r="E1064">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1065" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1065">
-        <v>250</v>
-      </c>
-      <c r="C1065">
-        <v>499</v>
-      </c>
-      <c r="D1065">
-        <v>1.19</v>
-      </c>
-      <c r="E1065">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1066" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1066" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1066">
-        <v>500</v>
-      </c>
-      <c r="C1066">
-        <v>999999</v>
-      </c>
-      <c r="D1066">
-        <v>0.92</v>
-      </c>
-      <c r="E1066">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1067" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1067" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1067">
-        <v>1</v>
-      </c>
-      <c r="C1067">
-        <v>49</v>
-      </c>
-      <c r="D1067">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1067">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1068" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1068" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1068">
-        <v>50</v>
-      </c>
-      <c r="C1068">
-        <v>99</v>
-      </c>
-      <c r="D1068">
-        <v>1.83</v>
-      </c>
-      <c r="E1068">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1069" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1069" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1069">
-        <v>100</v>
-      </c>
-      <c r="C1069">
-        <v>249</v>
-      </c>
-      <c r="D1069">
-        <v>1.47</v>
-      </c>
-      <c r="E1069">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1070" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1070" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1070">
-        <v>250</v>
-      </c>
-      <c r="C1070">
-        <v>499</v>
-      </c>
-      <c r="D1070">
-        <v>1.19</v>
-      </c>
-      <c r="E1070">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1071" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1071" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1071">
-        <v>500</v>
-      </c>
-      <c r="C1071">
-        <v>999999</v>
-      </c>
-      <c r="D1071">
-        <v>0.92</v>
-      </c>
-      <c r="E1071">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1072" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1072" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1072">
-        <v>1</v>
-      </c>
-      <c r="C1072">
-        <v>49</v>
-      </c>
-      <c r="D1072">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1072">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1073" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1073" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1073">
-        <v>50</v>
-      </c>
-      <c r="C1073">
-        <v>99</v>
-      </c>
-      <c r="D1073">
-        <v>1.83</v>
-      </c>
-      <c r="E1073">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1074" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1074" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1074">
-        <v>100</v>
-      </c>
-      <c r="C1074">
-        <v>249</v>
-      </c>
-      <c r="D1074">
-        <v>1.47</v>
-      </c>
-      <c r="E1074">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1075" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1075" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1075">
-        <v>250</v>
-      </c>
-      <c r="C1075">
-        <v>499</v>
-      </c>
-      <c r="D1075">
-        <v>1.19</v>
-      </c>
-      <c r="E1075">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1076" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1076" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1076">
-        <v>500</v>
-      </c>
-      <c r="C1076">
-        <v>999999</v>
-      </c>
-      <c r="D1076">
-        <v>0.92</v>
-      </c>
-      <c r="E1076">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1077" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1077" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1077">
-        <v>1</v>
-      </c>
-      <c r="C1077">
-        <v>49</v>
-      </c>
-      <c r="D1077">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1077">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1078" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1078" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1078">
-        <v>50</v>
-      </c>
-      <c r="C1078">
-        <v>99</v>
-      </c>
-      <c r="D1078">
-        <v>1.83</v>
-      </c>
-      <c r="E1078">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1079" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1079" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1079">
-        <v>100</v>
-      </c>
-      <c r="C1079">
-        <v>249</v>
-      </c>
-      <c r="D1079">
-        <v>1.47</v>
-      </c>
-      <c r="E1079">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1080" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1080" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1080">
-        <v>250</v>
-      </c>
-      <c r="C1080">
-        <v>499</v>
-      </c>
-      <c r="D1080">
-        <v>1.19</v>
-      </c>
-      <c r="E1080">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1081" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1081" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1081">
-        <v>500</v>
-      </c>
-      <c r="C1081">
-        <v>999999</v>
-      </c>
-      <c r="D1081">
-        <v>0.92</v>
-      </c>
-      <c r="E1081">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1082" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1082" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1082">
-        <v>1</v>
-      </c>
-      <c r="C1082">
-        <v>49</v>
-      </c>
-      <c r="D1082">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1082">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1083" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1083" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1083">
-        <v>50</v>
-      </c>
-      <c r="C1083">
-        <v>99</v>
-      </c>
-      <c r="D1083">
-        <v>1.83</v>
-      </c>
-      <c r="E1083">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1084" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1084" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1084">
-        <v>100</v>
-      </c>
-      <c r="C1084">
-        <v>249</v>
-      </c>
-      <c r="D1084">
-        <v>1.47</v>
-      </c>
-      <c r="E1084">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1085" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1085" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1085">
-        <v>250</v>
-      </c>
-      <c r="C1085">
-        <v>499</v>
-      </c>
-      <c r="D1085">
-        <v>1.19</v>
-      </c>
-      <c r="E1085">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1086" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1086" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1086">
-        <v>500</v>
-      </c>
-      <c r="C1086">
-        <v>999999</v>
-      </c>
-      <c r="D1086">
-        <v>0.92</v>
-      </c>
-      <c r="E1086">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="1087" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1087" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1087">
-        <v>1</v>
-      </c>
-      <c r="C1087">
-        <v>49</v>
-      </c>
-      <c r="D1087">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E1087">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1088" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1088" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1088">
-        <v>50</v>
-      </c>
-      <c r="C1088">
-        <v>99</v>
-      </c>
-      <c r="D1088">
-        <v>1.83</v>
-      </c>
-      <c r="E1088">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1089" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1089" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1089">
-        <v>100</v>
-      </c>
-      <c r="C1089">
-        <v>249</v>
-      </c>
-      <c r="D1089">
-        <v>1.47</v>
-      </c>
-      <c r="E1089">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1090" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1090" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1090">
-        <v>250</v>
-      </c>
-      <c r="C1090">
-        <v>499</v>
-      </c>
-      <c r="D1090">
-        <v>1.19</v>
-      </c>
-      <c r="E1090">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1091" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1091" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1091">
-        <v>500</v>
-      </c>
-      <c r="C1091">
-        <v>999999</v>
-      </c>
-      <c r="D1091">
-        <v>0.92</v>
-      </c>
-      <c r="E1091">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>